<commit_message>
Additional updates to include AGDD by last freeze, update the model_outputs file final cleanup of scripts
</commit_message>
<xml_diff>
--- a/model_outputs.xlsx
+++ b/model_outputs.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\R\freezing_tolerance\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\R\Endris_Rehm_2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1620C5A-F8A0-4A9F-AB61-6CA60F7AF747}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B117F774-E942-468E-8F8D-3D45D72203FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18930" yWindow="990" windowWidth="31020" windowHeight="19650" firstSheet="2" activeTab="4" xr2:uid="{A0FB6B5F-D5CF-4732-8622-D592A94C8237}"/>
+    <workbookView xWindow="24225" yWindow="525" windowWidth="23715" windowHeight="19185" firstSheet="2" activeTab="4" xr2:uid="{A0FB6B5F-D5CF-4732-8622-D592A94C8237}"/>
   </bookViews>
   <sheets>
     <sheet name="Climate" sheetId="4" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="822" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="817" uniqueCount="204">
   <si>
     <t>Estimate</t>
   </si>
@@ -597,9 +597,6 @@
     <t>Best selected model</t>
   </si>
   <si>
-    <t>year:Species</t>
-  </si>
-  <si>
     <t>Emmeans contrast on phenology</t>
   </si>
   <si>
@@ -636,13 +633,28 @@
     <t>phen3 - phen4</t>
   </si>
   <si>
-    <t>Emmeans contrast on species while accounting for year</t>
-  </si>
-  <si>
     <t>Best model:</t>
   </si>
   <si>
     <t>emmeans on species</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> contrast            estimate    SE  df t.ratio p.value</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> year2022 - year2023     1.83 0.513 193   3.565  0.0005</t>
+  </si>
+  <si>
+    <t>Emmeans contrast on species</t>
+  </si>
+  <si>
+    <t>Emmeans contrast on year</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> year2022 - year2023    -1.22 0.526 196  -2.322  0.0213</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> year2022 - year2023    -2.97 0.658 197  -4.513  &lt;.0001</t>
   </si>
 </sst>
 </file>
@@ -729,7 +741,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -753,6 +765,8 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1636,10 +1650,21 @@
   <dimension ref="A1:J33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+      <selection sqref="A1:J1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="2.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="6" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
@@ -2336,7 +2361,7 @@
   <dimension ref="A1:XFC84"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="A67" sqref="A67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2472,7 +2497,7 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="5" t="s">
         <v>176</v>
       </c>
     </row>
@@ -2937,7 +2962,7 @@
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="1" t="s">
+      <c r="A56" s="5" t="s">
         <v>169</v>
       </c>
       <c r="B56">
@@ -2957,7 +2982,7 @@
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="1" t="s">
+      <c r="A57" s="5" t="s">
         <v>170</v>
       </c>
       <c r="B57">
@@ -19733,10 +19758,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA1B2321-201B-4C4E-A277-72E73F958FBC}">
-  <dimension ref="A1:K46"/>
+  <dimension ref="A1:K45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A36" sqref="A36:A46"/>
+      <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19818,34 +19843,35 @@
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
+      <c r="A4" s="5">
         <v>8</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="4">
         <v>-13.5</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="G4">
+      <c r="F4" s="4"/>
+      <c r="G4" s="4">
         <v>10</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="4">
         <v>-575.91399999999999</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="4">
         <v>1172.9000000000001</v>
       </c>
-      <c r="J4">
+      <c r="J4" s="4">
         <v>1.1100000000000001</v>
       </c>
-      <c r="K4">
+      <c r="K4" s="4">
         <v>0.36299999999999999</v>
       </c>
     </row>
@@ -20106,7 +20132,7 @@
         <v>357.3</v>
       </c>
       <c r="E16">
-        <v>27.445</v>
+        <v>27.527000000000001</v>
       </c>
       <c r="F16" t="s">
         <v>67</v>
@@ -20129,10 +20155,10 @@
         <v>180</v>
       </c>
       <c r="E17">
-        <v>13.823</v>
+        <v>13.865</v>
       </c>
       <c r="F17">
-        <v>2.5900000000000001E-4</v>
+        <v>2.5300000000000002E-4</v>
       </c>
       <c r="G17" t="s">
         <v>5</v>
@@ -20152,463 +20178,378 @@
         <v>109.9</v>
       </c>
       <c r="E18">
-        <v>8.4410000000000007</v>
+        <v>8.4670000000000005</v>
       </c>
       <c r="F18">
-        <v>2.9999999999999997E-4</v>
+        <v>2.92E-4</v>
       </c>
       <c r="G18" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+      <c r="A19" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="B19">
+        <v>208</v>
+      </c>
+      <c r="C19">
+        <v>2699.7</v>
+      </c>
+      <c r="D19">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="7" t="s">
         <v>184</v>
       </c>
-      <c r="B19">
-        <v>2</v>
-      </c>
-      <c r="C19">
-        <v>17.899999999999999</v>
-      </c>
-      <c r="D19">
-        <v>9</v>
-      </c>
-      <c r="E19">
-        <v>0.68799999999999994</v>
-      </c>
-      <c r="F19">
-        <v>0.50349200000000005</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="B20">
-        <v>206</v>
-      </c>
-      <c r="C20">
-        <v>2681.8</v>
-      </c>
-      <c r="D20">
-        <v>13</v>
-      </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="7" t="s">
-        <v>185</v>
+      <c r="A22" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B22" t="s">
+        <v>164</v>
+      </c>
+      <c r="C22" t="s">
+        <v>165</v>
+      </c>
+      <c r="D22" t="s">
+        <v>22</v>
+      </c>
+      <c r="E22" t="s">
+        <v>166</v>
+      </c>
+      <c r="F22" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="B23" t="s">
-        <v>164</v>
-      </c>
-      <c r="C23" t="s">
-        <v>165</v>
-      </c>
-      <c r="D23" t="s">
-        <v>22</v>
-      </c>
-      <c r="E23" t="s">
-        <v>166</v>
-      </c>
-      <c r="F23" t="s">
-        <v>167</v>
+        <v>185</v>
+      </c>
+      <c r="B23" s="11">
+        <v>-1.7809999999999999</v>
+      </c>
+      <c r="C23" s="11">
+        <v>0.84499999999999997</v>
+      </c>
+      <c r="D23" s="12">
+        <v>193</v>
+      </c>
+      <c r="E23" s="11">
+        <v>-2.109</v>
+      </c>
+      <c r="F23">
+        <v>0.2205</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="B24">
-        <v>-1.74</v>
-      </c>
-      <c r="C24">
-        <v>0.85</v>
-      </c>
-      <c r="D24">
-        <v>191</v>
-      </c>
-      <c r="E24">
-        <v>-2.048</v>
-      </c>
-      <c r="F24">
-        <v>0.2475</v>
+      <c r="B24" s="11">
+        <v>-4.4340000000000002</v>
+      </c>
+      <c r="C24" s="11">
+        <v>0.70599999999999996</v>
+      </c>
+      <c r="D24" s="12">
+        <v>193</v>
+      </c>
+      <c r="E24" s="11">
+        <v>-6.2850000000000001</v>
+      </c>
+      <c r="F24" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="B25" s="11">
+        <v>-6.28</v>
+      </c>
+      <c r="C25" s="11">
+        <v>0.62</v>
+      </c>
+      <c r="D25" s="12">
+        <v>193</v>
+      </c>
+      <c r="E25" s="11">
+        <v>-10.129</v>
+      </c>
+      <c r="F25" t="s">
         <v>187</v>
-      </c>
-      <c r="B25">
-        <v>-4.4359999999999999</v>
-      </c>
-      <c r="C25">
-        <v>0.70699999999999996</v>
-      </c>
-      <c r="D25">
-        <v>191</v>
-      </c>
-      <c r="E25">
-        <v>-6.2770000000000001</v>
-      </c>
-      <c r="F25" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="B26">
-        <v>-6.2809999999999997</v>
-      </c>
-      <c r="C26">
-        <v>0.621</v>
-      </c>
-      <c r="D26">
-        <v>191</v>
-      </c>
-      <c r="E26">
-        <v>-10.114000000000001</v>
-      </c>
-      <c r="F26" t="s">
-        <v>188</v>
+      <c r="B26" s="11">
+        <v>-6.4020000000000001</v>
+      </c>
+      <c r="C26" s="11">
+        <v>1.595</v>
+      </c>
+      <c r="D26" s="12">
+        <v>193</v>
+      </c>
+      <c r="E26" s="11">
+        <v>-4.0129999999999999</v>
+      </c>
+      <c r="F26">
+        <v>8.0000000000000004E-4</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="B27">
-        <v>-6.5979999999999999</v>
-      </c>
-      <c r="C27">
-        <v>1.643</v>
-      </c>
-      <c r="D27">
-        <v>191</v>
-      </c>
-      <c r="E27">
-        <v>-4.0149999999999997</v>
+      <c r="B27" s="11">
+        <v>-2.653</v>
+      </c>
+      <c r="C27" s="11">
+        <v>0.96299999999999997</v>
+      </c>
+      <c r="D27" s="12">
+        <v>193</v>
+      </c>
+      <c r="E27" s="11">
+        <v>-2.7549999999999999</v>
       </c>
       <c r="F27">
-        <v>8.0000000000000004E-4</v>
+        <v>4.9799999999999997E-2</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="B28">
-        <v>-2.6960000000000002</v>
-      </c>
-      <c r="C28">
-        <v>0.96799999999999997</v>
-      </c>
-      <c r="D28">
-        <v>191</v>
-      </c>
-      <c r="E28">
-        <v>-2.7850000000000001</v>
-      </c>
-      <c r="F28">
-        <v>4.6100000000000002E-2</v>
+      <c r="B28" s="11">
+        <v>-4.4989999999999997</v>
+      </c>
+      <c r="C28" s="11">
+        <v>0.91500000000000004</v>
+      </c>
+      <c r="D28" s="12">
+        <v>193</v>
+      </c>
+      <c r="E28" s="11">
+        <v>-4.9160000000000004</v>
+      </c>
+      <c r="F28" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="B29">
-        <v>-4.5410000000000004</v>
-      </c>
-      <c r="C29">
-        <v>0.92</v>
-      </c>
-      <c r="D29">
-        <v>191</v>
-      </c>
-      <c r="E29">
-        <v>-4.9349999999999996</v>
-      </c>
-      <c r="F29" t="s">
-        <v>188</v>
+      <c r="B29" s="11">
+        <v>-4.6210000000000004</v>
+      </c>
+      <c r="C29" s="11">
+        <v>1.673</v>
+      </c>
+      <c r="D29" s="12">
+        <v>193</v>
+      </c>
+      <c r="E29" s="11">
+        <v>-2.762</v>
+      </c>
+      <c r="F29">
+        <v>4.8899999999999999E-2</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="B30">
-        <v>-4.859</v>
-      </c>
-      <c r="C30">
-        <v>1.7390000000000001</v>
-      </c>
-      <c r="D30">
-        <v>191</v>
-      </c>
-      <c r="E30">
-        <v>-2.794</v>
+      <c r="B30" s="11">
+        <v>-1.8460000000000001</v>
+      </c>
+      <c r="C30" s="11">
+        <v>0.78</v>
+      </c>
+      <c r="D30" s="12">
+        <v>193</v>
+      </c>
+      <c r="E30" s="11">
+        <v>-2.367</v>
       </c>
       <c r="F30">
-        <v>4.4999999999999998E-2</v>
+        <v>0.12889999999999999</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="B31">
-        <v>-1.845</v>
-      </c>
-      <c r="C31">
-        <v>0.78100000000000003</v>
-      </c>
-      <c r="D31">
-        <v>191</v>
-      </c>
-      <c r="E31">
-        <v>-2.3620000000000001</v>
+      <c r="B31" s="11">
+        <v>-1.9670000000000001</v>
+      </c>
+      <c r="C31" s="11">
+        <v>1.653</v>
+      </c>
+      <c r="D31" s="12">
+        <v>193</v>
+      </c>
+      <c r="E31" s="11">
+        <v>-1.19</v>
       </c>
       <c r="F31">
-        <v>0.13039999999999999</v>
+        <v>0.75719999999999998</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
+      <c r="A32" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="B32">
-        <v>-2.1629999999999998</v>
-      </c>
-      <c r="C32">
-        <v>1.7</v>
-      </c>
-      <c r="D32">
-        <v>191</v>
-      </c>
-      <c r="E32">
-        <v>-1.2729999999999999</v>
+      <c r="B32" s="11">
+        <v>-0.121</v>
+      </c>
+      <c r="C32" s="11">
+        <v>1.633</v>
+      </c>
+      <c r="D32" s="12">
+        <v>193</v>
+      </c>
+      <c r="E32" s="11">
+        <v>-7.3999999999999996E-2</v>
       </c>
       <c r="F32">
-        <v>0.70830000000000004</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="B33">
-        <v>-0.318</v>
-      </c>
-      <c r="C33">
-        <v>1.681</v>
-      </c>
-      <c r="D33">
-        <v>191</v>
-      </c>
-      <c r="E33">
-        <v>-0.189</v>
-      </c>
-      <c r="F33">
-        <v>0.99970000000000003</v>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="7" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="7" t="s">
-        <v>197</v>
+      <c r="A35" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B35" t="s">
+        <v>164</v>
+      </c>
+      <c r="C35" t="s">
+        <v>165</v>
+      </c>
+      <c r="D35" t="s">
+        <v>22</v>
+      </c>
+      <c r="E35" t="s">
+        <v>166</v>
+      </c>
+      <c r="F35" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>172</v>
+        <v>168</v>
+      </c>
+      <c r="B36">
+        <v>2.0270000000000001</v>
+      </c>
+      <c r="C36">
+        <v>0.6</v>
+      </c>
+      <c r="D36">
+        <v>15</v>
+      </c>
+      <c r="E36">
+        <v>3.3759999999999999</v>
+      </c>
+      <c r="F36">
+        <v>1.09E-2</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="B37" t="s">
-        <v>164</v>
-      </c>
-      <c r="C37" t="s">
-        <v>165</v>
-      </c>
-      <c r="D37" t="s">
-        <v>22</v>
-      </c>
-      <c r="E37" t="s">
-        <v>166</v>
-      </c>
-      <c r="F37" t="s">
-        <v>167</v>
+        <v>169</v>
+      </c>
+      <c r="B37">
+        <v>2.294</v>
+      </c>
+      <c r="C37">
+        <v>0.622</v>
+      </c>
+      <c r="D37">
+        <v>15</v>
+      </c>
+      <c r="E37">
+        <v>3.6909999999999998</v>
+      </c>
+      <c r="F37">
+        <v>5.7999999999999996E-3</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
-        <v>168</v>
+      <c r="A38" s="2" t="s">
+        <v>170</v>
       </c>
       <c r="B38">
-        <v>2.6619999999999999</v>
+        <v>0.26700000000000002</v>
       </c>
       <c r="C38">
-        <v>0.85</v>
+        <v>0.622</v>
       </c>
       <c r="D38">
         <v>15</v>
       </c>
       <c r="E38">
-        <v>3.1309999999999998</v>
+        <v>0.43</v>
       </c>
       <c r="F38">
-        <v>1.78E-2</v>
+        <v>0.90380000000000005</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="B39">
-        <v>2.9009999999999998</v>
-      </c>
-      <c r="C39">
-        <v>0.89300000000000002</v>
-      </c>
-      <c r="D39">
-        <v>15</v>
-      </c>
-      <c r="E39">
-        <v>3.2469999999999999</v>
-      </c>
-      <c r="F39">
-        <v>1.41E-2</v>
-      </c>
+      <c r="A39" s="1"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="B40">
-        <v>0.23799999999999999</v>
-      </c>
-      <c r="C40">
-        <v>0.89300000000000002</v>
-      </c>
-      <c r="D40">
-        <v>15</v>
-      </c>
-      <c r="E40">
-        <v>0.26700000000000002</v>
-      </c>
-      <c r="F40">
-        <v>0.96160000000000001</v>
+      <c r="A40" s="9" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="9"/>
+      <c r="A41" s="1" t="s">
+        <v>198</v>
+      </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="s">
-        <v>173</v>
+      <c r="A42" s="2" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="B43" t="s">
-        <v>164</v>
-      </c>
-      <c r="C43" t="s">
-        <v>165</v>
-      </c>
-      <c r="D43" t="s">
-        <v>22</v>
-      </c>
-      <c r="E43" t="s">
-        <v>166</v>
-      </c>
-      <c r="F43" t="s">
-        <v>167</v>
-      </c>
+      <c r="A43" s="1"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B44">
-        <v>1.3919999999999999</v>
-      </c>
-      <c r="C44">
-        <v>0.85</v>
-      </c>
-      <c r="D44">
-        <v>15</v>
-      </c>
-      <c r="E44">
-        <v>1.6359999999999999</v>
-      </c>
-      <c r="F44">
-        <v>0.26150000000000001</v>
-      </c>
+      <c r="A44" s="1"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="B45">
-        <v>1.714</v>
-      </c>
-      <c r="C45">
-        <v>0.86199999999999999</v>
-      </c>
-      <c r="D45">
-        <v>15</v>
-      </c>
-      <c r="E45">
-        <v>1.988</v>
-      </c>
-      <c r="F45">
-        <v>0.14949999999999999</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="B46">
-        <v>0.32200000000000001</v>
-      </c>
-      <c r="C46">
-        <v>0.86199999999999999</v>
-      </c>
-      <c r="D46">
-        <v>15</v>
-      </c>
-      <c r="E46">
-        <v>0.373</v>
-      </c>
-      <c r="F46">
-        <v>0.9264</v>
-      </c>
+      <c r="A45" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D6F133C-418D-4754-A9FA-2AE027867103}">
-  <dimension ref="A1:K50"/>
+  <dimension ref="A1:K56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A47" sqref="A47:A50"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25:A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20945,7 +20886,7 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -21028,7 +20969,7 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
@@ -21111,521 +21052,547 @@
         <v>0.86550000000000005</v>
       </c>
     </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="2"/>
+    </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="7" t="s">
+      <c r="A25" s="1" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="2"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="7" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="1"/>
-      <c r="B26" t="s">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" s="1"/>
+      <c r="B29" t="s">
         <v>18</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C29" t="s">
         <v>96</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D29" t="s">
         <v>62</v>
       </c>
-      <c r="E26" t="s">
+      <c r="E29" t="s">
         <v>20</v>
       </c>
-      <c r="F26" t="s">
+      <c r="F29" t="s">
         <v>65</v>
       </c>
-      <c r="G26" t="s">
+      <c r="G29" t="s">
         <v>22</v>
       </c>
-      <c r="H26" t="s">
+      <c r="H29" t="s">
         <v>23</v>
       </c>
-      <c r="I26" t="s">
+      <c r="I29" t="s">
         <v>24</v>
       </c>
-      <c r="J26" t="s">
+      <c r="J29" t="s">
         <v>25</v>
       </c>
-      <c r="K26" t="s">
+      <c r="K29" t="s">
         <v>26</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="1">
-        <v>16</v>
-      </c>
-      <c r="B27">
-        <v>-3583</v>
-      </c>
-      <c r="C27">
-        <v>9.5939999999999998E-2</v>
-      </c>
-      <c r="D27" t="s">
-        <v>28</v>
-      </c>
-      <c r="E27">
-        <v>1.77</v>
-      </c>
-      <c r="F27" t="s">
-        <v>28</v>
-      </c>
-      <c r="G27">
-        <v>9</v>
-      </c>
-      <c r="H27">
-        <v>-595.66300000000001</v>
-      </c>
-      <c r="I27">
-        <v>1210.2</v>
-      </c>
-      <c r="J27">
-        <v>0</v>
-      </c>
-      <c r="K27">
-        <v>0.59599999999999997</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="5">
-        <v>8</v>
-      </c>
-      <c r="B28" s="4">
-        <v>-2472</v>
-      </c>
-      <c r="C28" s="4">
-        <v>9.5939999999999998E-2</v>
-      </c>
-      <c r="D28" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E28" s="4">
-        <v>1.2210000000000001</v>
-      </c>
-      <c r="F28" s="4"/>
-      <c r="G28" s="4">
-        <v>7</v>
-      </c>
-      <c r="H28" s="4">
-        <v>-598.375</v>
-      </c>
-      <c r="I28" s="4">
-        <v>1211.3</v>
-      </c>
-      <c r="J28" s="4">
-        <v>1.0900000000000001</v>
-      </c>
-      <c r="K28" s="4">
-        <v>0.34499999999999997</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="1">
-        <v>4</v>
-      </c>
-      <c r="B29">
-        <v>-2.3730000000000002</v>
-      </c>
-      <c r="C29">
-        <v>9.418E-2</v>
-      </c>
-      <c r="D29" t="s">
-        <v>28</v>
-      </c>
-      <c r="G29">
-        <v>6</v>
-      </c>
-      <c r="H29">
-        <v>-601.32500000000005</v>
-      </c>
-      <c r="I29">
-        <v>1215.0999999999999</v>
-      </c>
-      <c r="J29">
-        <v>4.8499999999999996</v>
-      </c>
-      <c r="K29">
-        <v>5.2999999999999999E-2</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="B30">
-        <v>-2471</v>
+        <v>-3583</v>
       </c>
       <c r="C30">
         <v>9.5939999999999998E-2</v>
       </c>
+      <c r="D30" t="s">
+        <v>28</v>
+      </c>
       <c r="E30">
+        <v>1.77</v>
+      </c>
+      <c r="F30" t="s">
+        <v>28</v>
+      </c>
+      <c r="G30">
+        <v>9</v>
+      </c>
+      <c r="H30">
+        <v>-595.66300000000001</v>
+      </c>
+      <c r="I30">
+        <v>1210.2</v>
+      </c>
+      <c r="J30">
+        <v>0</v>
+      </c>
+      <c r="K30">
+        <v>0.59599999999999997</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" s="5">
+        <v>8</v>
+      </c>
+      <c r="B31" s="4">
+        <v>-2472</v>
+      </c>
+      <c r="C31" s="4">
+        <v>9.5939999999999998E-2</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E31" s="4">
         <v>1.2210000000000001</v>
       </c>
-      <c r="G30">
-        <v>5</v>
-      </c>
-      <c r="H30">
-        <v>-604.64700000000005</v>
-      </c>
-      <c r="I30">
-        <v>1219.5999999999999</v>
-      </c>
-      <c r="J30">
-        <v>9.3800000000000008</v>
-      </c>
-      <c r="K30">
-        <v>5.0000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="1">
-        <v>2</v>
-      </c>
-      <c r="B31">
-        <v>-1.1599999999999999</v>
-      </c>
-      <c r="C31">
-        <v>9.418E-2</v>
-      </c>
-      <c r="G31">
-        <v>4</v>
-      </c>
-      <c r="H31">
-        <v>-607.51</v>
-      </c>
-      <c r="I31">
-        <v>1223.2</v>
-      </c>
-      <c r="J31">
-        <v>13.01</v>
-      </c>
-      <c r="K31">
-        <v>1E-3</v>
+      <c r="F31" s="4"/>
+      <c r="G31" s="4">
+        <v>7</v>
+      </c>
+      <c r="H31" s="4">
+        <v>-598.375</v>
+      </c>
+      <c r="I31" s="4">
+        <v>1211.3</v>
+      </c>
+      <c r="J31" s="4">
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="K31" s="4">
+        <v>0.34499999999999997</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="B32">
-        <v>-2864</v>
+        <v>-2.3730000000000002</v>
+      </c>
+      <c r="C32">
+        <v>9.418E-2</v>
       </c>
       <c r="D32" t="s">
         <v>28</v>
       </c>
-      <c r="E32">
-        <v>1.419</v>
-      </c>
-      <c r="F32" t="s">
-        <v>28</v>
-      </c>
       <c r="G32">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H32">
-        <v>-627.66099999999994</v>
+        <v>-601.32500000000005</v>
       </c>
       <c r="I32">
-        <v>1272</v>
+        <v>1215.0999999999999</v>
       </c>
       <c r="J32">
-        <v>61.82</v>
+        <v>4.8499999999999996</v>
       </c>
       <c r="K32">
-        <v>0</v>
+        <v>5.2999999999999999E-2</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B33">
-        <v>-1752</v>
-      </c>
-      <c r="D33" t="s">
-        <v>28</v>
+        <v>-2471</v>
+      </c>
+      <c r="C33">
+        <v>9.5939999999999998E-2</v>
       </c>
       <c r="E33">
-        <v>0.86919999999999997</v>
+        <v>1.2210000000000001</v>
       </c>
       <c r="G33">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H33">
-        <v>-630.56100000000004</v>
+        <v>-604.64700000000005</v>
       </c>
       <c r="I33">
-        <v>1273.5</v>
+        <v>1219.5999999999999</v>
       </c>
       <c r="J33">
-        <v>63.32</v>
+        <v>9.3800000000000008</v>
       </c>
       <c r="K33">
-        <v>0</v>
+        <v>5.0000000000000001E-3</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B34">
-        <v>5.444</v>
-      </c>
-      <c r="D34" t="s">
-        <v>28</v>
+        <v>-1.1599999999999999</v>
+      </c>
+      <c r="C34">
+        <v>9.418E-2</v>
       </c>
       <c r="G34">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H34">
-        <v>-631.98400000000004</v>
+        <v>-607.51</v>
       </c>
       <c r="I34">
-        <v>1274.3</v>
+        <v>1223.2</v>
       </c>
       <c r="J34">
-        <v>64.05</v>
+        <v>13.01</v>
       </c>
       <c r="K34">
-        <v>0</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="B35">
-        <v>-1751</v>
+        <v>-2864</v>
+      </c>
+      <c r="D35" t="s">
+        <v>28</v>
       </c>
       <c r="E35">
-        <v>0.86919999999999997</v>
+        <v>1.419</v>
+      </c>
+      <c r="F35" t="s">
+        <v>28</v>
       </c>
       <c r="G35">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="H35">
-        <v>-635.64499999999998</v>
+        <v>-627.66099999999994</v>
       </c>
       <c r="I35">
-        <v>1279.5</v>
+        <v>1272</v>
       </c>
       <c r="J35">
-        <v>69.28</v>
+        <v>61.82</v>
       </c>
       <c r="K35">
         <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A36" s="2">
-        <v>1</v>
+      <c r="A36" s="1">
+        <v>7</v>
       </c>
       <c r="B36">
-        <v>6.657</v>
+        <v>-1752</v>
+      </c>
+      <c r="D36" t="s">
+        <v>28</v>
+      </c>
+      <c r="E36">
+        <v>0.86919999999999997</v>
       </c>
       <c r="G36">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="H36">
-        <v>-637.05499999999995</v>
+        <v>-630.56100000000004</v>
       </c>
       <c r="I36">
-        <v>1280.2</v>
+        <v>1273.5</v>
       </c>
       <c r="J36">
-        <v>70.02</v>
+        <v>63.32</v>
       </c>
       <c r="K36">
         <v>0</v>
       </c>
     </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
+        <v>3</v>
+      </c>
+      <c r="B37">
+        <v>5.444</v>
+      </c>
+      <c r="D37" t="s">
+        <v>28</v>
+      </c>
+      <c r="G37">
+        <v>5</v>
+      </c>
+      <c r="H37">
+        <v>-631.98400000000004</v>
+      </c>
+      <c r="I37">
+        <v>1274.3</v>
+      </c>
+      <c r="J37">
+        <v>64.05</v>
+      </c>
+      <c r="K37">
+        <v>0</v>
+      </c>
+    </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A38" s="7" t="s">
+      <c r="A38" s="1">
+        <v>5</v>
+      </c>
+      <c r="B38">
+        <v>-1751</v>
+      </c>
+      <c r="E38">
+        <v>0.86919999999999997</v>
+      </c>
+      <c r="G38">
+        <v>4</v>
+      </c>
+      <c r="H38">
+        <v>-635.64499999999998</v>
+      </c>
+      <c r="I38">
+        <v>1279.5</v>
+      </c>
+      <c r="J38">
+        <v>69.28</v>
+      </c>
+      <c r="K38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A39" s="2">
+        <v>1</v>
+      </c>
+      <c r="B39">
+        <v>6.657</v>
+      </c>
+      <c r="G39">
+        <v>3</v>
+      </c>
+      <c r="H39">
+        <v>-637.05499999999995</v>
+      </c>
+      <c r="I39">
+        <v>1280.2</v>
+      </c>
+      <c r="J39">
+        <v>70.02</v>
+      </c>
+      <c r="K39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A41" s="7" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A42" s="1"/>
+      <c r="B42" t="s">
+        <v>145</v>
+      </c>
+      <c r="C42" t="s">
+        <v>155</v>
+      </c>
+      <c r="D42" t="s">
+        <v>156</v>
+      </c>
+      <c r="E42" t="s">
+        <v>157</v>
+      </c>
+      <c r="F42" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B43">
+        <v>1</v>
+      </c>
+      <c r="C43">
+        <v>1221.0999999999999</v>
+      </c>
+      <c r="D43">
+        <v>1221.0999999999999</v>
+      </c>
+      <c r="E43">
+        <v>82.218999999999994</v>
+      </c>
+      <c r="F43" t="s">
+        <v>67</v>
+      </c>
+      <c r="G43" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B44">
+        <v>1</v>
+      </c>
+      <c r="C44">
+        <v>80.099999999999994</v>
+      </c>
+      <c r="D44">
+        <v>80.099999999999994</v>
+      </c>
+      <c r="E44">
+        <v>5.391</v>
+      </c>
+      <c r="F44">
+        <v>2.1190000000000001E-2</v>
+      </c>
+      <c r="G44" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B45">
+        <v>2</v>
+      </c>
+      <c r="C45">
+        <v>165.1</v>
+      </c>
+      <c r="D45">
+        <v>82.6</v>
+      </c>
+      <c r="E45">
+        <v>5.5590000000000002</v>
+      </c>
+      <c r="F45">
+        <v>4.4400000000000004E-3</v>
+      </c>
+      <c r="G45" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="B46">
+        <v>211</v>
+      </c>
+      <c r="C46">
+        <v>3133.9</v>
+      </c>
+      <c r="D46">
+        <v>14.9</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="10" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B50" t="s">
+        <v>164</v>
+      </c>
+      <c r="C50" t="s">
+        <v>165</v>
+      </c>
+      <c r="D50" t="s">
+        <v>22</v>
+      </c>
+      <c r="E50" t="s">
+        <v>166</v>
+      </c>
+      <c r="F50" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B51">
+        <v>-2.0270000000000001</v>
+      </c>
+      <c r="C51">
+        <v>0.64200000000000002</v>
+      </c>
+      <c r="D51">
+        <v>15</v>
+      </c>
+      <c r="E51">
+        <v>-3.1560000000000001</v>
+      </c>
+      <c r="F51">
+        <v>1.6899999999999998E-2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="B52">
+        <v>-1.6120000000000001</v>
+      </c>
+      <c r="C52">
+        <v>0.64200000000000002</v>
+      </c>
+      <c r="D52">
+        <v>15</v>
+      </c>
+      <c r="E52">
+        <v>-2.5099999999999998</v>
+      </c>
+      <c r="F52">
+        <v>5.8900000000000001E-2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="B53">
+        <v>0.41499999999999998</v>
+      </c>
+      <c r="C53">
+        <v>0.64200000000000002</v>
+      </c>
+      <c r="D53">
+        <v>15</v>
+      </c>
+      <c r="E53">
+        <v>0.64600000000000002</v>
+      </c>
+      <c r="F53">
+        <v>0.79759999999999998</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A39" s="1"/>
-      <c r="B39" t="s">
-        <v>145</v>
-      </c>
-      <c r="C39" t="s">
-        <v>155</v>
-      </c>
-      <c r="D39" t="s">
-        <v>156</v>
-      </c>
-      <c r="E39" t="s">
-        <v>157</v>
-      </c>
-      <c r="F39" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="B40">
-        <v>1</v>
-      </c>
-      <c r="C40">
-        <v>1221.0999999999999</v>
-      </c>
-      <c r="D40">
-        <v>1221.0999999999999</v>
-      </c>
-      <c r="E40">
-        <v>82.218999999999994</v>
-      </c>
-      <c r="F40" t="s">
-        <v>67</v>
-      </c>
-      <c r="G40" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B41">
-        <v>1</v>
-      </c>
-      <c r="C41">
-        <v>80.099999999999994</v>
-      </c>
-      <c r="D41">
-        <v>80.099999999999994</v>
-      </c>
-      <c r="E41">
-        <v>5.391</v>
-      </c>
-      <c r="F41">
-        <v>2.1190000000000001E-2</v>
-      </c>
-      <c r="G41" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="B42">
-        <v>2</v>
-      </c>
-      <c r="C42">
-        <v>165.1</v>
-      </c>
-      <c r="D42">
-        <v>82.6</v>
-      </c>
-      <c r="E42">
-        <v>5.5590000000000002</v>
-      </c>
-      <c r="F42">
-        <v>4.4400000000000004E-3</v>
-      </c>
-      <c r="G42" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A43" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="B43">
-        <v>211</v>
-      </c>
-      <c r="C43">
-        <v>3133.9</v>
-      </c>
-      <c r="D43">
-        <v>14.9</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A46" s="10" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A47" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="B47" t="s">
-        <v>164</v>
-      </c>
-      <c r="C47" t="s">
-        <v>165</v>
-      </c>
-      <c r="D47" t="s">
-        <v>22</v>
-      </c>
-      <c r="E47" t="s">
-        <v>166</v>
-      </c>
-      <c r="F47" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A48" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B48">
-        <v>-2.0270000000000001</v>
-      </c>
-      <c r="C48">
-        <v>0.64200000000000002</v>
-      </c>
-      <c r="D48">
-        <v>15</v>
-      </c>
-      <c r="E48">
-        <v>-3.1560000000000001</v>
-      </c>
-      <c r="F48">
-        <v>1.6899999999999998E-2</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="B49">
-        <v>-1.6120000000000001</v>
-      </c>
-      <c r="C49">
-        <v>0.64200000000000002</v>
-      </c>
-      <c r="D49">
-        <v>15</v>
-      </c>
-      <c r="E49">
-        <v>-2.5099999999999998</v>
-      </c>
-      <c r="F49">
-        <v>5.8900000000000001E-2</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="B50">
-        <v>0.41499999999999998</v>
-      </c>
-      <c r="C50">
-        <v>0.64200000000000002</v>
-      </c>
-      <c r="D50">
-        <v>15</v>
-      </c>
-      <c r="E50">
-        <v>0.64600000000000002</v>
-      </c>
-      <c r="F50">
-        <v>0.79759999999999998</v>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" s="2" t="s">
+        <v>202</v>
       </c>
     </row>
   </sheetData>

</xml_diff>